<commit_message>
Most up to date tests
</commit_message>
<xml_diff>
--- a/10MTests/10MeterTests.xlsx
+++ b/10MTests/10MeterTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KholySa\OneDrive\Documents\HS Osnabruck\Tests\10MTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDDEE76-7C59-4427-B37B-882FD6634D72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4159AFCC-A0B0-472E-9CD9-44DE30B358D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -723,16 +723,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -742,10 +755,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -753,6 +765,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -764,24 +782,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1099,7 +1099,7 @@
   <dimension ref="B1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1118,116 +1118,116 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="11" t="s">
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5" t="s">
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="22" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="8"/>
+      <c r="M3" s="23"/>
     </row>
     <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="15"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="29"/>
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="26" t="s">
+      <c r="L5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="M5" s="32"/>
+      <c r="M5" s="19"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1237,10 +1237,10 @@
         <v>46</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="9" t="s">
         <v>41</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -1250,16 +1250,16 @@
         <v>47</v>
       </c>
       <c r="K6" s="2"/>
-      <c r="L6" s="27" t="s">
+      <c r="L6" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="33"/>
+      <c r="M6" s="20"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="9" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1271,10 +1271,10 @@
       <c r="F7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="9" t="s">
         <v>31</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1286,599 +1286,599 @@
       <c r="K7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="27" t="s">
+      <c r="L7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="33"/>
+      <c r="M7" s="20"/>
     </row>
     <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="L8" s="28" t="s">
+      <c r="L8" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="34"/>
+      <c r="M8" s="21"/>
     </row>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="18"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="34"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="G10" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="L10" s="26" t="s">
+      <c r="L10" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="M10" s="32"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="21"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="33"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="20"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="21"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="9"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="33"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="20"/>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="34"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="21"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="18"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="34"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="J15" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="K15" s="19" t="s">
+      <c r="K15" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="L15" s="26" t="s">
+      <c r="L15" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="M15" s="32"/>
+      <c r="M15" s="19"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="21"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="21"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="9"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="33"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="20"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="21"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="21"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="9"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="33"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="20"/>
     </row>
     <row r="18" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="34"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="21"/>
     </row>
     <row r="19" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="18"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="34"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="G20" s="26" t="s">
+      <c r="G20" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I20" s="19" t="s">
+      <c r="I20" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="J20" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="K20" s="19" t="s">
+      <c r="K20" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="L20" s="26" t="s">
+      <c r="L20" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="M20" s="32"/>
+      <c r="M20" s="19"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="21"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="21"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="9"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="33"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="20"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="21"/>
+      <c r="C22" s="9"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="21"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="9"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="33"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="20"/>
     </row>
     <row r="23" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="34"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="21"/>
     </row>
     <row r="24" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="18"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="34"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="32"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="19"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="21"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="21"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="9"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="33"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="20"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="21"/>
+      <c r="C27" s="9"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="21"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="9"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="33"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="20"/>
     </row>
     <row r="28" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="34"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="21"/>
     </row>
     <row r="29" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="18"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="34"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="32"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="19"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="21"/>
+      <c r="C31" s="9"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="21"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="9"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="33"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="20"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="21"/>
+      <c r="C32" s="9"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="21"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="9"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="33"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="20"/>
     </row>
     <row r="33" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="34"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="21"/>
     </row>
     <row r="34" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="18"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="34"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="26"/>
-      <c r="M35" s="32"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="19"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="21"/>
+      <c r="C36" s="9"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="21"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="9"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="L36" s="27"/>
-      <c r="M36" s="33"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="20"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="21"/>
+      <c r="C37" s="9"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="21"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="9"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="33"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="20"/>
     </row>
     <row r="38" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="34"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="B24:M24"/>
+    <mergeCell ref="B19:M19"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B29:M29"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="B24:M24"/>
-    <mergeCell ref="B19:M19"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B29:M29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Most up to date tests"
This reverts commit a4791ec60369a3f97df928ae4b66aca7f8eb4658.
</commit_message>
<xml_diff>
--- a/10MTests/10MeterTests.xlsx
+++ b/10MTests/10MeterTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KholySa\OneDrive\Documents\HS Osnabruck\Tests\10MTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4159AFCC-A0B0-472E-9CD9-44DE30B358D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDDEE76-7C59-4427-B37B-882FD6634D72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -723,29 +723,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -755,9 +742,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -765,12 +753,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -782,6 +764,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1099,7 +1099,7 @@
   <dimension ref="B1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1118,116 +1118,116 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="30" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="22" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="23"/>
+      <c r="M3" s="8"/>
     </row>
     <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="29"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="15"/>
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="M5" s="19"/>
+      <c r="M5" s="32"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="21" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1237,10 +1237,10 @@
         <v>46</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="21" t="s">
         <v>41</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -1250,16 +1250,16 @@
         <v>47</v>
       </c>
       <c r="K6" s="2"/>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="20"/>
+      <c r="M6" s="33"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="21" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1271,10 +1271,10 @@
       <c r="F7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="21" t="s">
         <v>31</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1286,599 +1286,599 @@
       <c r="K7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="L7" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="20"/>
+      <c r="M7" s="33"/>
     </row>
     <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="21"/>
+      <c r="M8" s="34"/>
     </row>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="34"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="18"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="M10" s="19"/>
+      <c r="M10" s="32"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="9"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="21"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="20"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="33"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="9"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="21"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="20"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="33"/>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="34"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="34"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="18"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="K15" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="L15" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="M15" s="19"/>
+      <c r="M15" s="32"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="9"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="21"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="20"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="33"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="9"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="21"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="20"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="33"/>
     </row>
     <row r="18" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="21"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="34"/>
     </row>
     <row r="19" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="34"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="18"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="I20" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="J20" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="K20" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="L20" s="13" t="s">
+      <c r="L20" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="M20" s="19"/>
+      <c r="M20" s="32"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="9"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="9"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="20"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="33"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="9"/>
+      <c r="C22" s="21"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="9"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="21"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="20"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="33"/>
     </row>
     <row r="23" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="21"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="34"/>
     </row>
     <row r="24" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="34"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="18"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="32"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="9"/>
+      <c r="C26" s="21"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="9"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="21"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="20"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="33"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="9"/>
+      <c r="C27" s="21"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="9"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="21"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="20"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="33"/>
     </row>
     <row r="28" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="21"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="34"/>
     </row>
     <row r="29" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="34"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="18"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="19"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="32"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="9"/>
+      <c r="C31" s="21"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="9"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="21"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="20"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="33"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="9"/>
+      <c r="C32" s="21"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="9"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="21"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="20"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="33"/>
     </row>
     <row r="33" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="21"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="34"/>
     </row>
     <row r="34" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="34"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="18"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="19"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="32"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="9"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="9"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="21"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="20"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="33"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="9"/>
+      <c r="C37" s="21"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="9"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="21"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="20"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="33"/>
     </row>
     <row r="38" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="21"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="B9:M9"/>
     <mergeCell ref="B14:M14"/>
     <mergeCell ref="B24:M24"/>
     <mergeCell ref="B19:M19"/>
     <mergeCell ref="B34:M34"/>
     <mergeCell ref="B29:M29"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="B9:M9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>